<commit_message>
ran benches with training size of 100 to test performance against training size 10
</commit_message>
<xml_diff>
--- a/notebooks/data/saved data/benchmarks.xlsx
+++ b/notebooks/data/saved data/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A65451-FD1E-A046-9F6E-FF800AFED882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCA90B7-4516-574F-9FE2-D414B6F0EEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{9A2CFE81-F432-D54B-820E-AEEC0E972080}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="9" xr2:uid="{9A2CFE81-F432-D54B-820E-AEEC0E972080}"/>
   </bookViews>
   <sheets>
     <sheet name="bio2" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="spring" sheetId="7" r:id="rId7"/>
     <sheet name="opt" sheetId="8" r:id="rId8"/>
     <sheet name="graphs" sheetId="9" r:id="rId9"/>
+    <sheet name="All_benchs" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="bio2__1" localSheetId="0">'bio2'!$A$1:$L$58</definedName>
@@ -70,10 +71,28 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1214876E-0B41-EF4A-A393-F4BA49B53F59}</author>
+  </authors>
+  <commentList>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Should we try uniform distribution?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{FFD2D342-4AAA-B247-9AD5-194FD2977A63}" name="bio2" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/bio2" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/bio2" comma="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -91,7 +110,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{4B102954-4406-3F4A-AF39-10D02CB4DB97}" name="fhn" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/fhn" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/fhn" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -102,7 +121,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{82790430-4F5E-4F45-8108-BB28ED80A16D}" name="lalo20" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/lalo20" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/lalo20" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -118,7 +137,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{421100B9-3254-5C40-867C-E16206EAA73F}" name="pendulum" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/pendulum" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/pendulum" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -129,7 +148,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{7C488245-6FD9-B940-9F51-9C49041D9A6B}" name="prde20" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/prde20" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/prde20" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -141,7 +160,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{626A21AA-C26F-C54E-A524-105A3C7D3BB7}" name="robe21" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/robe21" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/robe21" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -153,7 +172,7 @@
     </textPr>
   </connection>
   <connection id="7" xr16:uid="{8A48B3F5-F77B-054D-8918-C7EC62427C01}" name="spring" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/spring" comma="1">
+    <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/spring" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -169,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="36">
   <si>
     <t>train_size</t>
   </si>
@@ -272,6 +291,12 @@
   <si>
     <t>spring</t>
   </si>
+  <si>
+    <t>Avg Mse</t>
+  </si>
+  <si>
+    <t>Train time (s)</t>
+  </si>
 </sst>
 </file>
 
@@ -312,10 +337,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3296,7 +3324,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4204,6 +4232,1278 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sampling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> period</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> vs MSE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-EG"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>bio2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'bio2'!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>8.3781399171079901E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0753834187405099E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0633987456818499</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.0255816548267299E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2.9279904623369102E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>5.5713435385320605E-7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2.5207966606136798E-6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>4.8897761833380202E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2588626697247901E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>fhn</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fhn!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.31316068814773</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2475543855858899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.19098923701653</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9881195219854803E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10854789589682</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7759633680295305E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.70261174188019E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11634094226083901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11409089402136099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>lalo20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lalo20!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.134915225906106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4346365082530205E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12844138024201099</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>3.7755397927367499E-7</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>3.2791208063830799E-7</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>3.40612615334752E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6478905646583801E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1.2503803945039599E-5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2.9969311177646799E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>pendulum</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pendulum!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.11261197128165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.09442544599255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0344239380128999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7525303360104599E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91788421551402</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57157825540176299</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.739800623088961</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59045494444090696</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70372900782007897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>prde20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>prde20!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>14.145598903482901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0622632852295</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8201247365617603E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7040635924938896E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2298774398577308</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1838633791292708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0654108315174007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.22193146468167E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.523961690619559</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>robe21</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>robe21!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0373645802621701E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0323105433830702E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0243347323596599E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0085911046684401E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9776210185718901E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9624264804636801E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.88904894689426E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7528866303520199E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5112043662328E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>spring</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pendulum!$A$14:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>spring!$C$14:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.2098689499387</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9946020341320197E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.3999551795924101E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>1.4420200354975E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.6744176546945</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>5.1871915311733402E-8</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1.69860950024758E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.27641065113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-EAA8-694E-8B02-AA73A8710F6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1316099247"/>
+        <c:axId val="812962560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1316099247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. of observables</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-EG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-EG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812962560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="812962560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-EG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-EG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1316099247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-EG"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-EG"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4325,6 +5625,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6432,6 +7772,544 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6586,6 +8464,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>559405</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>75595</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1951D69B-83F0-D74D-A2D9-E26E541E6B98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6931,12 +8847,20 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A10" dT="2022-09-25T22:06:45.63" personId="{A80F9E15-0FE4-5148-BBCB-4203E8481853}" id="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
+    <text>Should we try uniform distribution?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A16246-F289-8546-8A6D-57D59BA2DFBC}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8852,12 +10776,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEC0487-BEB8-9545-BFB5-9A7FE013F84C}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>20.814</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.0255816548267299E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>18.484000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.9881195219854803E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>18.907</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.7755397927367499E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>19.731000000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.7525303360104599E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>12.311999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7.7040635924938896E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>13.526</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.0085911046684401E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>23.276</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.3999551795924101E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCA4501-898C-854B-9A9E-A03118D06649}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9727,8 +11757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6630EC-BC96-1041-98F2-A1F90D33235E}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11348,8 +13378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619E9799-89C9-4C4E-8B43-AEE9690C3483}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12232,8 +14262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F62091-A1A6-9D4C-9EAA-202B02307759}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13253,8 +15283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F1ACFD-17EA-7A45-8E80-CE31E1E0D769}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14295,8 +16325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7046A9AC-213D-1C4D-A5AF-4C047DE16A46}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15519,7 +17549,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -15530,7 +17560,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -15539,7 +17569,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
@@ -15550,7 +17580,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -15559,7 +17589,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
@@ -15570,7 +17600,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -15579,7 +17609,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
@@ -15590,7 +17620,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -15599,7 +17629,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
@@ -15610,7 +17640,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -15619,7 +17649,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
@@ -15630,7 +17660,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -15639,7 +17669,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
@@ -15650,7 +17680,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -15677,8 +17707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5100C7DA-3C7C-2C40-B1FA-7B01A869E85A}">
   <dimension ref="G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A10" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
created new trn benchmark
</commit_message>
<xml_diff>
--- a/notebooks/data/saved data/benchmarks.xlsx
+++ b/notebooks/data/saved data/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBEF06E-B5BB-FE40-936E-7B5944AC13BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B7EBC5-7BE1-0646-9A2F-63854F2BEB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="9" xr2:uid="{9A2CFE81-F432-D54B-820E-AEEC0E972080}"/>
   </bookViews>
@@ -25,16 +25,25 @@
     <sheet name="All_benchs" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="benches" localSheetId="9">All_benchs!$L$3:$N$9</definedName>
-    <definedName name="benches_1" localSheetId="9">All_benchs!$C$3:$E$11</definedName>
-    <definedName name="benches_2" localSheetId="9">All_benchs!$F$3:$H$9</definedName>
-    <definedName name="benches_3" localSheetId="9">All_benchs!$H$12:$J$19</definedName>
-    <definedName name="benches_4" localSheetId="9">All_benchs!$D$12:$F$19</definedName>
+    <definedName name="benches" localSheetId="9">All_benchs!$L$4:$N$10</definedName>
+    <definedName name="benches_1" localSheetId="9">All_benchs!$C$4:$E$12</definedName>
+    <definedName name="benches_2" localSheetId="9">All_benchs!$F$4:$H$10</definedName>
+    <definedName name="benches_3" localSheetId="9">All_benchs!$H$13:$J$20</definedName>
+    <definedName name="benches_4" localSheetId="9">All_benchs!$D$13:$F$20</definedName>
+    <definedName name="benches_5" localSheetId="9">All_benchs!$L$13:$N$20</definedName>
+    <definedName name="benches_6" localSheetId="9">All_benchs!$D$24:$F$31</definedName>
+    <definedName name="benches_7" localSheetId="9">All_benchs!$H$24:$J$31</definedName>
+    <definedName name="benches_8" localSheetId="9">All_benchs!$L$24:$N$27</definedName>
+    <definedName name="benches_9" localSheetId="9">All_benchs!$G$34:$I$37</definedName>
+    <definedName name="bio2_" localSheetId="0">'bio2'!$A$60:$L$71</definedName>
     <definedName name="bio2__1" localSheetId="0">'bio2'!$A$1:$L$58</definedName>
     <definedName name="fhn_1" localSheetId="1">fhn!$A$1:$E$58</definedName>
     <definedName name="lalo20_1" localSheetId="2">lalo20!$A$1:$J$58</definedName>
+    <definedName name="pendulum" localSheetId="3">pendulum!$G$1:$K$12</definedName>
     <definedName name="pendulum_1" localSheetId="3">pendulum!$A$1:$E$58</definedName>
+    <definedName name="prde20" localSheetId="4">prde20!$H$1:$M$12</definedName>
     <definedName name="prde20_1" localSheetId="4">prde20!$A$1:$F$58</definedName>
+    <definedName name="robe21" localSheetId="5">robe21!$H$1:$M$24</definedName>
     <definedName name="robe21_1" localSheetId="5">robe21!$A$1:$F$58</definedName>
     <definedName name="spring_1" localSheetId="6">spring!$A$1:$G$58</definedName>
   </definedNames>
@@ -82,7 +91,7 @@
     <author>tc={1214876E-0B41-EF4A-A393-F4BA49B53F59}</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -141,7 +150,52 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{FFD2D342-4AAA-B247-9AD5-194FD2977A63}" name="bio2" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="6" xr16:uid="{C4BEF0A6-430B-0F47-B8FC-6257CC4643A1}" name="benches5" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/benches" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{EECB1460-DAC4-0C41-B9BE-3A17FCF37201}" name="benches6" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/benches" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" xr16:uid="{E04C1C6E-0FF6-F340-A0CA-64115F2AEC9D}" name="benches7" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/benches" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" xr16:uid="{29ABFA20-5224-9148-9E82-D4CF44A2DFC8}" name="benches8" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/benches" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" xr16:uid="{B7E94110-3111-8C46-8617-83E4F73701BF}" name="benches9" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/benches" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" xr16:uid="{FFD2D342-4AAA-B247-9AD5-194FD2977A63}" name="bio2" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/bio2" comma="1">
       <textFields count="12">
         <textField/>
@@ -159,7 +213,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{4B102954-4406-3F4A-AF39-10D02CB4DB97}" name="fhn" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="12" xr16:uid="{EACDE40F-54CD-B747-BD2A-3BFB48C30873}" name="bio21" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/bio2" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="13" xr16:uid="{4B102954-4406-3F4A-AF39-10D02CB4DB97}" name="fhn" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/fhn" comma="1">
       <textFields count="5">
         <textField/>
@@ -170,7 +242,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" xr16:uid="{82790430-4F5E-4F45-8108-BB28ED80A16D}" name="lalo20" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="14" xr16:uid="{82790430-4F5E-4F45-8108-BB28ED80A16D}" name="lalo20" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/lalo20" comma="1">
       <textFields count="10">
         <textField/>
@@ -186,7 +258,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" xr16:uid="{421100B9-3254-5C40-867C-E16206EAA73F}" name="pendulum" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="15" xr16:uid="{421100B9-3254-5C40-867C-E16206EAA73F}" name="pendulum" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/pendulum" comma="1">
       <textFields count="5">
         <textField/>
@@ -197,7 +269,18 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" xr16:uid="{7C488245-6FD9-B940-9F51-9C49041D9A6B}" name="prde20" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="16" xr16:uid="{68F7FF9E-7879-1A4A-BEFB-3AD61DD86F4C}" name="pendulum1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/pendulum" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="17" xr16:uid="{7C488245-6FD9-B940-9F51-9C49041D9A6B}" name="prde20" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/prde20" comma="1">
       <textFields count="6">
         <textField/>
@@ -209,7 +292,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" xr16:uid="{626A21AA-C26F-C54E-A524-105A3C7D3BB7}" name="robe21" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="18" xr16:uid="{A7F92517-C977-2D45-A77C-0494C5D24B31}" name="prde201" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/prde20" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="19" xr16:uid="{626A21AA-C26F-C54E-A524-105A3C7D3BB7}" name="robe21" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/saved data/robe21" comma="1">
       <textFields count="6">
         <textField/>
@@ -221,7 +316,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" xr16:uid="{8A48B3F5-F77B-054D-8918-C7EC62427C01}" name="spring" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="20" xr16:uid="{E9D0C5F6-57D7-8D40-A357-087198EB599A}" name="robe211" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/robe21" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="21" xr16:uid="{8A48B3F5-F77B-054D-8918-C7EC62427C01}" name="spring" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/b6062805/Documents/Koopman/AutoKoopman/notebooks/data/spring" comma="1">
       <textFields count="7">
         <textField/>
@@ -238,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="47">
   <si>
     <t>train_size</t>
   </si>
@@ -374,6 +481,12 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Training size: 50</t>
+  </si>
+  <si>
+    <t>Training size: 10</t>
+  </si>
 </sst>
 </file>
 
@@ -408,10 +521,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,62 +1253,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Training size vs MSE</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-EG"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1575,10 +1632,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pendulum!$A$2:$A$10</c:f>
+              <c:f>pendulum!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1605,16 +1662,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pendulum!$C$2:$C$10</c:f>
+              <c:f>pendulum!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>1.3555211489450899E-3</c:v>
                 </c:pt>
@@ -1641,6 +1701,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.2993071550882501E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1.0837163637585199E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,10 +1787,10 @@
             <c:numRef>
               <c:f>prde20!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.3421326243976902E-2</c:v>
+                  <c:v>1.5897274628366001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.7040635924938896E-3</c:v>
@@ -1735,25 +1798,25 @@
                 <c:pt idx="2">
                   <c:v>3.5135931677729697E-4</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
+                <c:pt idx="3">
                   <c:v>2.2256880640810398E-5</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
+                <c:pt idx="4">
                   <c:v>3.80609937643308E-6</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
+                <c:pt idx="5">
                   <c:v>4.90439659309425E-6</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
+                <c:pt idx="6">
                   <c:v>6.50814860594338E-5</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
+                <c:pt idx="7">
                   <c:v>6.3208261354168899E-7</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.00E+00">
+                <c:pt idx="8">
                   <c:v>5.1593379939635101E-6</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.00E+00">
+                <c:pt idx="9">
                   <c:v>4.0188142178210999E-6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1843,34 +1906,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.7817371844688101E-2</c:v>
+                  <c:v>2.4782660918956999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0085911046684401E-2</c:v>
+                  <c:v>1.9324391684173201E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74247550956764996</c:v>
+                  <c:v>8.7988426826244803E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>2.5410582321080499E-7</c:v>
+                  <c:v>3.19226922647052E-7</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1.5939653612533399E-8</c:v>
+                  <c:v>1.7522400323843001E-8</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>4.6972948565812797E-8</c:v>
+                  <c:v>5.5999430765217997E-8</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>4.26467676534149E-8</c:v>
+                  <c:v>1.9186071020638699E-8</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>6.9236922058669997E-8</c:v>
+                  <c:v>1.6783838274772099E-8</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1.30610456274233E-8</c:v>
+                  <c:v>2.2563624080300701E-8</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>3.2532684239582901E-8</c:v>
+                  <c:v>2.1558196923545701E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2019,20 +2082,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2040,20 +2089,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1000">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
                   <a:t>Training Size</a:t>
                 </a:r>
               </a:p>
@@ -2080,16 +2132,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-EG"/>
@@ -2146,20 +2198,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2167,20 +2205,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1000">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
                   <a:t> MSE</a:t>
                 </a:r>
               </a:p>
@@ -2207,23 +2248,23 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-EG"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2274,6 +2315,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1771461567304087"/>
+          <c:y val="2.179962928369459E-2"/>
+          <c:w val="0.75618372703412073"/>
+          <c:h val="5.2553045560244351E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8332,13 +8383,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>385629</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190262</xdr:rowOff>
+      <xdr:colOff>391809</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>202659</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8406,15 +8457,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>147807</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>196985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>132921</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123040</xdr:rowOff>
+      <xdr:colOff>268028</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28466</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8443,16 +8494,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>193744</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>559405</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>75595</xdr:rowOff>
+      <xdr:colOff>802597</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>89106</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8489,51 +8540,87 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="bio2__1" connectionId="6" xr16:uid="{23AE6D99-FCE9-EC4B-B726-69E4CD573B99}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="bio2" connectionId="12" xr16:uid="{56759CB2-501E-5B4D-8C3F-11AB3E4C6326}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="robe21_1" connectionId="19" xr16:uid="{52663BBD-1BDF-9F45-BB83-FBF53FBF3FA5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="spring_1" connectionId="21" xr16:uid="{9FA49B94-5873-E841-BFE2-215514590169}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_9" connectionId="10" xr16:uid="{F332228F-E560-414E-BE76-F296A5DC747A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_8" connectionId="9" xr16:uid="{E8E45296-F838-F042-A3A0-9B27DAE6B39C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_7" connectionId="8" xr16:uid="{30A92188-A05D-3E4B-B183-B071A6A12171}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_6" connectionId="7" xr16:uid="{0063ACEE-4131-2048-8003-97ABC6B56DF8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_5" connectionId="6" xr16:uid="{EB0D265A-688B-6543-B7DE-812625C022AD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_4" connectionId="5" xr16:uid="{91D9A886-8B5B-D149-AAC7-7CDA2670365B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_3" connectionId="4" xr16:uid="{EA2CB22C-2614-6F43-A2E8-D01C7E6C5BFD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_2" connectionId="3" xr16:uid="{FBF67DC1-47D9-F043-8CB2-7E3358D200EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="bio2__1" connectionId="11" xr16:uid="{23AE6D99-FCE9-EC4B-B726-69E4CD573B99}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_1" connectionId="2" xr16:uid="{310508FF-9BE3-C146-B41A-DB0D0FA006FA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches" connectionId="1" xr16:uid="{023B07EF-D609-A243-ABFA-6C24A28C4F5B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fhn_1" connectionId="7" xr16:uid="{74922FBB-5EFF-BB40-9893-9F6FCC49B556}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lalo20_1" connectionId="8" xr16:uid="{1C812D5A-5621-174C-B67E-4C30AE8337BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fhn_1" connectionId="13" xr16:uid="{74922FBB-5EFF-BB40-9893-9F6FCC49B556}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pendulum_1" connectionId="9" xr16:uid="{1E26A177-E7E2-9C4B-9187-77FE7EB81C2D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lalo20_1" connectionId="14" xr16:uid="{1C812D5A-5621-174C-B67E-4C30AE8337BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="prde20_1" connectionId="10" xr16:uid="{271A936F-50AF-364D-ACC3-92DDEBE3C9FE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pendulum" connectionId="16" xr16:uid="{71223DD0-6F3F-384F-B6EC-D91AD246F734}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="robe21_1" connectionId="11" xr16:uid="{52663BBD-1BDF-9F45-BB83-FBF53FBF3FA5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pendulum_1" connectionId="15" xr16:uid="{1E26A177-E7E2-9C4B-9187-77FE7EB81C2D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="spring_1" connectionId="12" xr16:uid="{9FA49B94-5873-E841-BFE2-215514590169}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="prde20" connectionId="18" xr16:uid="{130CB578-C5CF-2F48-85A7-49A09B53158F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_4" connectionId="5" xr16:uid="{91D9A886-8B5B-D149-AAC7-7CDA2670365B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="prde20_1" connectionId="17" xr16:uid="{271A936F-50AF-364D-ACC3-92DDEBE3C9FE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benches_3" connectionId="4" xr16:uid="{EA2CB22C-2614-6F43-A2E8-D01C7E6C5BFD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="robe21" connectionId="20" xr16:uid="{0578E6FD-6E23-784E-9587-926167C7FF46}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8841,7 +8928,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A11" dT="2022-09-25T22:06:45.63" personId="{A80F9E15-0FE4-5148-BBCB-4203E8481853}" id="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
+  <threadedComment ref="A12" dT="2022-09-25T22:06:45.63" personId="{A80F9E15-0FE4-5148-BBCB-4203E8481853}" id="{1214876E-0B41-EF4A-A393-F4BA49B53F59}">
     <text>Should we try uniform distribution?</text>
   </threadedComment>
 </ThreadedComments>
@@ -8849,17 +8936,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A16246-F289-8546-8A6D-57D59BA2DFBC}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8906,7 +8993,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>13.401999999999999</v>
+        <v>9.6479999999999997</v>
       </c>
       <c r="C2" s="1">
         <v>4.1013521489282301E-5</v>
@@ -8944,7 +9031,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>20.814</v>
+        <v>15.750999999999999</v>
       </c>
       <c r="C3" s="1">
         <v>1.0255816548267299E-6</v>
@@ -8982,7 +9069,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>39.872</v>
+        <v>32.975000000000001</v>
       </c>
       <c r="C4" s="1">
         <v>3.86600947030818E-7</v>
@@ -9020,7 +9107,7 @@
         <v>50</v>
       </c>
       <c r="B5">
-        <v>71.912000000000006</v>
+        <v>60.53</v>
       </c>
       <c r="C5" s="1">
         <v>1.1948917503797301E-6</v>
@@ -9058,7 +9145,7 @@
         <v>75</v>
       </c>
       <c r="B6">
-        <v>102.938</v>
+        <v>88.897999999999996</v>
       </c>
       <c r="C6" s="1">
         <v>2.6906021473205901E-7</v>
@@ -9096,7 +9183,7 @@
         <v>100</v>
       </c>
       <c r="B7">
-        <v>134.64599999999999</v>
+        <v>117.75700000000001</v>
       </c>
       <c r="C7" s="1">
         <v>2.52218285067131E-7</v>
@@ -9134,7 +9221,7 @@
         <v>125</v>
       </c>
       <c r="B8">
-        <v>162.99100000000001</v>
+        <v>147.04300000000001</v>
       </c>
       <c r="C8" s="1">
         <v>3.69539858772581E-7</v>
@@ -9172,7 +9259,7 @@
         <v>150</v>
       </c>
       <c r="B9">
-        <v>199.11099999999999</v>
+        <v>175.68299999999999</v>
       </c>
       <c r="C9" s="1">
         <v>3.1674594357591901E-7</v>
@@ -9210,7 +9297,7 @@
         <v>175</v>
       </c>
       <c r="B10">
-        <v>233.96700000000001</v>
+        <v>202.92699999999999</v>
       </c>
       <c r="C10" s="1">
         <v>1.84503331134511E-6</v>
@@ -9248,7 +9335,7 @@
         <v>200</v>
       </c>
       <c r="B11">
-        <v>261.11799999999999</v>
+        <v>232.827</v>
       </c>
       <c r="C11" s="1">
         <v>1.0338507786183999E-7</v>
@@ -10762,6 +10849,125 @@
       <c r="L57" s="1">
         <v>5.5299049497542204E-7</v>
       </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+    </row>
+    <row r="68" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+    </row>
+    <row r="70" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10770,539 +10976,942 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEC0487-BEB8-9545-BFB5-9A7FE013F84C}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="10" width="12.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="3"/>
-    <col min="17" max="17" width="19.5" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="19.5" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="E2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="M1" s="6" t="s">
+      <c r="K2" s="5"/>
+      <c r="M2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="2">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="2">
         <v>1.919</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E4" s="3">
         <v>6.9008039548734202E-4</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="2">
         <v>5.048</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H4" s="3">
         <v>1456.69823962644</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J4" s="2">
         <v>20.814</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K4" s="3">
         <v>1.0255816548267299E-6</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M4" s="2">
         <v>643.28099999999995</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N4" s="3">
         <v>1.4493556003627901</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="2">
         <v>0.20899999999999999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E5" s="3">
         <v>0.357936903139979</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G5" s="4">
         <v>0.76700000000000002</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="3">
         <v>0.19170763517171399</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J5" s="2">
         <v>18.484000000000002</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K5" s="3">
         <v>4.9881195219854803E-4</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M5" s="2">
         <v>635.17200000000003</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N5" s="3">
         <v>0.53083404230738795</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="2">
         <v>0.24</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="3">
         <v>6.0986222329937603E-3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="2">
         <v>2.2509999999999999</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H6" s="3">
         <v>8.2993048134017307E-6</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J6" s="2">
         <v>18.907</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K6" s="3">
         <v>3.7755397927367499E-7</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M6" s="2">
         <v>627.9</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N6" s="3">
         <v>7.8781219839307894E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="2">
         <v>1.151</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="3">
         <v>2.4230038475313801E-2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G7" s="2">
         <v>1.7010000000000001</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="3">
         <v>2.4502122533164701E-2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J7" s="2">
         <v>19.731000000000002</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K7" s="3">
         <v>1.7525303360104599E-4</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M7" s="2">
         <v>630.50699999999995</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N7" s="3">
         <v>6.1972863562051499E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="2">
         <v>0.22800000000000001</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="3">
         <v>2.0649717581940901</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G8" s="2">
         <v>0.94599999999999995</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J8" s="2">
         <v>12.311999999999999</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K8" s="3">
         <v>7.7040635924938896E-3</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M8" s="2">
         <v>628.76099999999997</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N8" s="3">
         <v>1.5306236687214601</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="2">
         <v>0.70399999999999996</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="3">
         <v>9.73672904149922E-4</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="2">
         <v>1.476</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H9" s="3">
         <v>2.53530432891391E-2</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J9" s="2">
         <v>13.526</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K9" s="3">
         <v>2.0085911046684401E-2</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M9" s="2">
         <v>631.95600000000002</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N9" s="3">
         <v>1.34249722301498E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="2">
         <v>0.26</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="3">
         <v>18.640764969386499</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="2">
         <v>1.228</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="3">
         <v>16.304422966382798</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J10" s="2">
         <v>23.276</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K10" s="3">
         <v>1.3999551795924101E-6</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M10" s="2">
         <v>628.04399999999998</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N10" s="3">
         <v>1.7055096032568301E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D11" s="6" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="H11" s="6" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="H12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="L11" s="6" t="s">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="L12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5" t="s">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="L13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B14" s="4">
         <v>9</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="4">
         <v>3.2559999999999998</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="3">
         <v>1456.69823962644</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="6">
         <v>446075489.90734202</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H14" s="4">
         <v>13.045999999999999</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I14" s="3">
         <v>1.0255816548267299E-6</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J14" s="6">
         <v>2.6460074553547801E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="L14" s="4">
+        <v>626.93299999999999</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.58094721181810205</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.281321519747259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="4">
         <v>0.69199999999999995</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E15" s="3">
         <v>0.19170763517171399</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="6">
         <v>2.7450596337604201</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H15" s="4">
         <v>11.798</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I15" s="3">
         <v>4.9881195219854803E-4</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J15" s="6">
         <v>3.8630563799333099E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="L15" s="4">
+        <v>629.48400000000004</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0.22229626969108299</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1.55078061309774</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B16" s="4">
         <v>7</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D16" s="4">
         <v>2.1320000000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E16" s="3">
         <v>8.2993048134017307E-6</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="6">
         <v>2.1873774335978802E-3</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H16" s="4">
         <v>12.734999999999999</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I16" s="3">
         <v>3.7755397927367499E-7</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J16" s="6">
         <v>5.3894361500447005E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="L16" s="4">
+        <v>630.49</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1.91369676769443E-2</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.116778010945621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E17" s="3">
         <v>2.4502122533164701E-2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F17" s="6">
         <v>0.92515031583623997</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H17" s="4">
         <v>11.997</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I17" s="3">
         <v>1.7525303360104599E-4</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J17" s="6">
         <v>0.113406185235697</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="L17" s="4">
+        <v>636.56500000000005</v>
+      </c>
+      <c r="M17" s="3">
+        <v>8.9522902241490995E-2</v>
+      </c>
+      <c r="N17" s="6">
+        <v>2.1031449253008798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B18" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="4">
         <v>0.89600000000000002</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H18" s="4">
         <v>13.526</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I18" s="3">
         <v>1.23637779277552E-3</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J18" s="6">
         <v>8.4238188802768899E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="L18" s="4">
+        <v>637.05899999999997</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1.0329357187141801</v>
+      </c>
+      <c r="N18" s="6">
+        <v>1.6305574114154799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B19" s="4">
         <v>3</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D19" s="4">
         <v>0.9</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="3">
         <v>2.53530432891391E-2</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F19" s="6">
         <v>0.62963451270389303</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="4">
         <v>12.032999999999999</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I19" s="3">
         <v>1.9324391684173201E-2</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J19" s="6">
         <v>0.40437490605912602</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="L19" s="4">
+        <v>633.21199999999999</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1.63796467281164E-3</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.19854538443835701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B20" s="4">
         <v>4</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="4">
         <v>1.109</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E20" s="3">
         <v>16.304422966382798</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="6">
         <v>41212.945782985298</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H20" s="4">
         <v>13.185</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I20" s="3">
         <v>1.3999551795924101E-6</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J20" s="6">
         <v>9.4966445729602993E-3</v>
       </c>
+      <c r="L20" s="4">
+        <v>616.98500000000001</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1.6596401733687802E-2</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.69797354165547698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10.523</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1450.10797931876</v>
+      </c>
+      <c r="F25" s="6">
+        <v>447163326.76259297</v>
+      </c>
+      <c r="H25" s="4">
+        <v>54.344999999999999</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1.1948917503797301E-6</v>
+      </c>
+      <c r="J25" s="6">
+        <v>1.7647503698847101E-4</v>
+      </c>
+      <c r="L25" s="4">
+        <v>2525.5360000000001</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.29711130423019699</v>
+      </c>
+      <c r="N25" s="6">
+        <v>0.37054484956810402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3.1080000000000001</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.140460530471161</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4.4892715964419496</v>
+      </c>
+      <c r="H26" s="4">
+        <v>52.176000000000002</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.29800355582722E-6</v>
+      </c>
+      <c r="J26" s="6">
+        <v>4.9918362138803001E-3</v>
+      </c>
+      <c r="L26" s="4">
+        <v>2504.7739999999999</v>
+      </c>
+      <c r="M26" s="3">
+        <v>6.8246604447812304E-2</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.57039514669499003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="4">
+        <v>7</v>
+      </c>
+      <c r="D27" s="4">
+        <v>7.6420000000000003</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.0209952670833301E-7</v>
+      </c>
+      <c r="F27" s="6">
+        <v>4.73047254357724E-4</v>
+      </c>
+      <c r="H27" s="4">
+        <v>52.709000000000003</v>
+      </c>
+      <c r="I27" s="3">
+        <v>7.7541650172936501E-8</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2.5811653407706498E-4</v>
+      </c>
+      <c r="L27" s="4">
+        <v>2509.4659999999999</v>
+      </c>
+      <c r="M27" s="3">
+        <v>7.0137094449486299E-3</v>
+      </c>
+      <c r="N27" s="6">
+        <v>7.6225764699010795E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3.2909999999999999</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3.0192803098460199E-2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1.15717793229003</v>
+      </c>
+      <c r="H28" s="4">
+        <v>52.16</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2.1745466582459799E-4</v>
+      </c>
+      <c r="J28" s="6">
+        <v>6.0063444891228598E-2</v>
+      </c>
+      <c r="L28" s="4">
+        <v>2465.0079999999998</v>
+      </c>
+      <c r="M28" s="3">
+        <v>3.4852276803135303E-2</v>
+      </c>
+      <c r="N28" s="6">
+        <v>1.3258091020006499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="4">
+        <v>3</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3.6930000000000001</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="4">
+        <v>51.329000000000001</v>
+      </c>
+      <c r="I29" s="3">
+        <v>6.5030584948908102E-6</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0.19509164014321501</v>
+      </c>
+      <c r="L29" s="4">
+        <v>2484.4009999999998</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1.69923469515572</v>
+      </c>
+      <c r="N29" s="6">
+        <v>1.0920159399076901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3.7050000000000001</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1.6303837142838201E-2</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.36909839184412802</v>
+      </c>
+      <c r="H30" s="4">
+        <v>50.753</v>
+      </c>
+      <c r="I30" s="3">
+        <v>3.19226922647052E-7</v>
+      </c>
+      <c r="J30" s="6">
+        <v>1.8229036213875699E-3</v>
+      </c>
+      <c r="L30" s="4">
+        <v>2489.154</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1.12301520151925E-4</v>
+      </c>
+      <c r="N30" s="6">
+        <v>6.1760005342992703E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4.5250000000000004</v>
+      </c>
+      <c r="E31" s="3">
+        <v>16.316331644794701</v>
+      </c>
+      <c r="F31" s="6">
+        <v>41453.069006783597</v>
+      </c>
+      <c r="H31" s="4">
+        <v>52.034999999999997</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3.9105385986558302E-6</v>
+      </c>
+      <c r="J31" s="6">
+        <v>7.8491697257044701E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="M1:N1"/>
+  <mergeCells count="13">
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="A22:N22"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11313,7 +11922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCA4501-898C-854B-9A9E-A03118D06649}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -13803,10 +14412,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619E9799-89C9-4C4E-8B43-AEE9690C3483}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G1" sqref="G1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13815,9 +14424,13 @@
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13834,7 +14447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
@@ -13851,7 +14464,7 @@
         <v>2.4087007413881299E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -13867,8 +14480,9 @@
       <c r="E3">
         <v>3.0026119811572198E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>25</v>
       </c>
@@ -13884,8 +14498,11 @@
       <c r="E4" s="1">
         <v>9.3363489859106302E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50</v>
       </c>
@@ -13901,8 +14518,9 @@
       <c r="E5">
         <v>3.7513662640415899E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
@@ -13918,8 +14536,11 @@
       <c r="E6" s="1">
         <v>9.2526363000309798E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -13935,8 +14556,11 @@
       <c r="E7" s="1">
         <v>7.2261584434548003E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
@@ -13952,8 +14576,11 @@
       <c r="E8" s="1">
         <v>9.9354149321089399E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>150</v>
       </c>
@@ -13969,8 +14596,11 @@
       <c r="E9" s="1">
         <v>7.3615352864304798E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>175</v>
       </c>
@@ -13986,8 +14616,9 @@
       <c r="E10">
         <v>2.16223818020199E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
@@ -14003,8 +14634,9 @@
       <c r="E11">
         <v>1.7788318718911899E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -14021,7 +14653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.01</v>
       </c>
@@ -14038,7 +14670,7 @@
         <v>2.11298623906313</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -14055,7 +14687,7 @@
         <v>2.0761232599034098</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.05</v>
       </c>
@@ -14687,10 +15319,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F62091-A1A6-9D4C-9EAA-202B02307759}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14699,10 +15331,14 @@
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -14721,34 +15357,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>6.9509999999999996</v>
-      </c>
-      <c r="C2">
-        <v>3.3421326243976902E-2</v>
+        <v>12.895</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.5897274628366001E-2</v>
       </c>
       <c r="D2">
-        <v>5.2559203646515798E-2</v>
+        <v>2.5130791052408199E-2</v>
       </c>
       <c r="E2">
-        <v>2.7516036606779402E-2</v>
+        <v>1.3130976036561401E-2</v>
       </c>
       <c r="F2">
-        <v>2.0188738478635501E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9.4300567961283898E-3</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>12.311999999999999</v>
-      </c>
-      <c r="C3">
+        <v>21.021000000000001</v>
+      </c>
+      <c r="C3" s="1">
         <v>7.7040635924938896E-3</v>
       </c>
       <c r="D3">
@@ -14760,15 +15397,16 @@
       <c r="F3">
         <v>4.5681465403275704E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>25.841000000000001</v>
-      </c>
-      <c r="C4">
+        <v>41.508000000000003</v>
+      </c>
+      <c r="C4" s="1">
         <v>3.5135931677729697E-4</v>
       </c>
       <c r="D4">
@@ -14780,13 +15418,14 @@
       <c r="F4">
         <v>2.0357798849649099E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>51.155999999999999</v>
+        <v>74.709999999999994</v>
       </c>
       <c r="C5" s="1">
         <v>2.2256880640810398E-5</v>
@@ -14800,13 +15439,17 @@
       <c r="F5" s="1">
         <v>1.30777018541742E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
       <c r="B6">
-        <v>76.322000000000003</v>
+        <v>105.489</v>
       </c>
       <c r="C6" s="1">
         <v>3.80609937643308E-6</v>
@@ -14820,13 +15463,17 @@
       <c r="F6" s="1">
         <v>1.97340459998399E-6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
-        <v>98.203999999999994</v>
+        <v>138.709</v>
       </c>
       <c r="C7" s="1">
         <v>4.90439659309425E-6</v>
@@ -14840,18 +15487,22 @@
       <c r="F7" s="1">
         <v>2.5719745344709099E-6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
       <c r="B8">
-        <v>122.4</v>
+        <v>170.01599999999999</v>
       </c>
       <c r="C8" s="1">
         <v>6.50814860594338E-5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>1.02482797744907E-4</v>
       </c>
       <c r="E8" s="1">
@@ -14860,13 +15511,16 @@
       <c r="F8" s="1">
         <v>9.8052412837605705E-7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>150</v>
       </c>
       <c r="B9">
-        <v>144.51400000000001</v>
+        <v>198.88499999999999</v>
       </c>
       <c r="C9" s="1">
         <v>6.3208261354168899E-7</v>
@@ -14880,13 +15534,17 @@
       <c r="F9" s="1">
         <v>2.16902409973379E-7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>175</v>
       </c>
       <c r="B10">
-        <v>168.268</v>
+        <v>222.45400000000001</v>
       </c>
       <c r="C10" s="1">
         <v>5.1593379939635101E-6</v>
@@ -14900,13 +15558,17 @@
       <c r="F10" s="1">
         <v>2.8304340400944199E-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
       <c r="B11">
-        <v>194.28800000000001</v>
+        <v>267.27</v>
       </c>
       <c r="C11" s="1">
         <v>4.0188142178210999E-6</v>
@@ -14920,8 +15582,12 @@
       <c r="F11" s="1">
         <v>2.1132264071458401E-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -14941,7 +15607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.01</v>
       </c>
@@ -14961,7 +15627,7 @@
         <v>15.046718042187701</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -14981,7 +15647,7 @@
         <v>14.891435118112801</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.05</v>
       </c>
@@ -15708,10 +16374,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F1ACFD-17EA-7A45-8E80-CE31E1E0D769}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N23" sqref="H1:N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15720,9 +16386,13 @@
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15742,207 +16412,237 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>7.2960000000000003</v>
+        <v>14.981999999999999</v>
       </c>
       <c r="C2">
-        <v>2.7817371844688101E-2</v>
+        <v>2.4782660918956999E-2</v>
       </c>
       <c r="D2">
-        <v>4.1450059148569897E-2</v>
+        <v>3.3798849490633102E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>4.7954884026330599E-6</v>
+        <v>3.4736269759550798E-6</v>
       </c>
       <c r="F2">
-        <v>4.1997260897091798E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4.0545659639262099E-2</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>13.526</v>
+        <v>20.143000000000001</v>
       </c>
       <c r="C3">
-        <v>2.0085911046684401E-2</v>
+        <v>1.9324391684173201E-2</v>
       </c>
       <c r="D3">
-        <v>2.99558438186938E-2</v>
+        <v>2.7007487831202801E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>3.5383521773777101E-6</v>
+        <v>3.0765340999386E-6</v>
       </c>
       <c r="F3">
-        <v>3.0298350969182101E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.0962610687216799E-2</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>28.067</v>
+        <v>38.615000000000002</v>
       </c>
       <c r="C4">
-        <v>0.74247550956764996</v>
+        <v>8.7988426826244803E-2</v>
       </c>
       <c r="D4">
-        <v>0.60205750170239603</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.2822746301006001</v>
+        <v>6.4914637515760099E-2</v>
+      </c>
+      <c r="E4">
+        <v>9.7431309147719705E-2</v>
       </c>
       <c r="F4">
-        <v>0.34309439689995302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.101619333815254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>53.866999999999997</v>
+        <v>72.733999999999995</v>
       </c>
       <c r="C5" s="1">
-        <v>2.5410582321080499E-7</v>
+        <v>3.19226922647052E-7</v>
       </c>
       <c r="D5" s="1">
-        <v>3.7819513939834999E-7</v>
+        <v>4.7654459582356298E-7</v>
       </c>
       <c r="E5" s="1">
-        <v>5.0505663264263299E-11</v>
+        <v>2.4579096293458201E-10</v>
       </c>
       <c r="F5" s="1">
-        <v>3.8407182457080001E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4.8089038115466003E-7</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
       <c r="B6">
-        <v>75.429000000000002</v>
+        <v>107.753</v>
       </c>
       <c r="C6" s="1">
-        <v>1.5939653612533399E-8</v>
+        <v>1.7522400323843001E-8</v>
       </c>
       <c r="D6" s="1">
-        <v>2.3497182706011001E-8</v>
+        <v>2.5862242099314899E-8</v>
       </c>
       <c r="E6" s="1">
-        <v>2.1925624534133501E-11</v>
+        <v>4.64342668262476E-11</v>
       </c>
       <c r="F6" s="1">
-        <v>2.42998525070551E-8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.6658524605387899E-8</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
-        <v>102.128</v>
+        <v>142.22499999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>4.6972948565812797E-8</v>
+        <v>5.5999430765217997E-8</v>
       </c>
       <c r="D7" s="1">
-        <v>6.9650622310678303E-8</v>
+        <v>8.3082921477528504E-8</v>
       </c>
       <c r="E7" s="1">
-        <v>2.9149684448812803E-11</v>
+        <v>4.1695543281815899E-11</v>
       </c>
       <c r="F7" s="1">
-        <v>7.1239073702311499E-8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.4873675274843697E-8</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
       <c r="B8">
-        <v>127.381</v>
+        <v>172.97900000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>4.26467676534149E-8</v>
+        <v>1.9186071020638699E-8</v>
       </c>
       <c r="D8" s="1">
-        <v>6.31981465840855E-8</v>
+        <v>2.84888133143735E-8</v>
       </c>
       <c r="E8" s="1">
-        <v>2.71181116812609E-11</v>
+        <v>1.4783636709764401E-11</v>
       </c>
       <c r="F8" s="1">
-        <v>6.4715038264478004E-8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.90546161108328E-8</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>150</v>
       </c>
       <c r="B9">
-        <v>154.96899999999999</v>
+        <v>208.874</v>
       </c>
       <c r="C9" s="1">
-        <v>6.9236922058669997E-8</v>
+        <v>1.6783838274772099E-8</v>
       </c>
       <c r="D9" s="1">
-        <v>1.02588481478278E-7</v>
+        <v>2.4886010749686999E-8</v>
       </c>
       <c r="E9" s="1">
-        <v>3.3860979167531199E-11</v>
+        <v>1.6173605082601601E-11</v>
       </c>
       <c r="F9" s="1">
-        <v>1.05088423718563E-7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.54493304695467E-8</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>175</v>
       </c>
       <c r="B10">
-        <v>180.393</v>
+        <v>246.762</v>
       </c>
       <c r="C10" s="1">
-        <v>1.30610456274233E-8</v>
+        <v>2.2563624080300701E-8</v>
       </c>
       <c r="D10" s="1">
-        <v>1.9335293531709701E-8</v>
+        <v>3.3476954910619699E-8</v>
       </c>
       <c r="E10" s="1">
-        <v>1.9053173864497099E-11</v>
+        <v>1.5213049238837701E-11</v>
       </c>
       <c r="F10" s="1">
-        <v>1.9828790176695799E-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.4198704281043499E-8</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
       <c r="B11">
-        <v>204.69</v>
+        <v>286.411</v>
       </c>
       <c r="C11" s="1">
-        <v>3.2532684239582901E-8</v>
+        <v>2.1558196923545701E-8</v>
       </c>
       <c r="D11" s="1">
-        <v>4.8122749066421699E-8</v>
+        <v>3.1908937455535399E-8</v>
       </c>
       <c r="E11" s="1">
-        <v>3.1637695383615699E-11</v>
+        <v>2.4138838397199501E-11</v>
       </c>
       <c r="F11" s="1">
-        <v>4.9443665956943299E-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.2741514476704498E-8</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -15962,7 +16662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.01</v>
       </c>
@@ -15981,8 +16681,9 @@
       <c r="F14">
         <v>3.08749522725064E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -16001,8 +16702,9 @@
       <c r="F15">
         <v>3.07740665986929E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.05</v>
       </c>
@@ -16022,7 +16724,7 @@
         <v>3.0611950953114201E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.1</v>
       </c>
@@ -16041,8 +16743,12 @@
       <c r="F17">
         <v>3.0298350969182101E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.2</v>
       </c>
@@ -16061,8 +16767,12 @@
       <c r="F18">
         <v>2.96964654892506E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.25</v>
       </c>
@@ -16081,8 +16791,12 @@
       <c r="F19">
         <v>2.9405769341725001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.5</v>
       </c>
@@ -16101,8 +16815,12 @@
       <c r="F20">
         <v>2.8037314331814299E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -16121,8 +16839,12 @@
       <c r="F21">
         <v>2.5619310814225301E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -16141,11 +16863,19 @@
       <c r="F22">
         <v>2.15753425401475E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -16165,7 +16895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -16185,7 +16915,7 @@
         <v>3.0298350969182101E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -16205,7 +16935,7 @@
         <v>2.9871168844327601E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -16225,10 +16955,10 @@
         <v>1.541732443136E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -16248,7 +16978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -16268,7 +16998,7 @@
         <v>3.0298350969182101E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -16288,7 +17018,7 @@
         <v>3.0106895552047801E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -17976,7 +18706,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -17987,7 +18717,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -17996,7 +18726,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
@@ -18007,7 +18737,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -18016,7 +18746,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
@@ -18027,7 +18757,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -18036,7 +18766,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
@@ -18047,7 +18777,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -18056,7 +18786,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
@@ -18067,7 +18797,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -18076,7 +18806,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
@@ -18087,7 +18817,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -18096,7 +18826,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
@@ -18107,7 +18837,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -18134,7 +18864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5100C7DA-3C7C-2C40-B1FA-7B01A869E85A}">
   <dimension ref="G2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>